<commit_message>
Added LED matrix connectors
</commit_message>
<xml_diff>
--- a/docs/shopping_list.xlsx
+++ b/docs/shopping_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\PoF_2015\Setups\211123_TWT_jet_grid\Electronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\project-TWT-jetting-grid\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263FF32B-1F02-4904-89AC-462100B8EFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D89E6A-62D8-44FB-BA70-E75143C62272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26325" windowHeight="16395" xr2:uid="{6ACBF970-17D1-4E70-A647-E338031FE07A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26318" windowHeight="16395" xr2:uid="{6ACBF970-17D1-4E70-A647-E338031FE07A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="165">
   <si>
     <t>https://www.omega.nl/pptst/PXM309.html</t>
   </si>
@@ -289,18 +289,6 @@
     <t>Phoenix 1424137</t>
   </si>
   <si>
-    <t>Phoenix 1440151</t>
-  </si>
-  <si>
-    <t>https://nl.farnell.com/phoenix-contact/sacc-m12-kd-nut-sh/emc-hexagonal-nut-m12/dp/3286565</t>
-  </si>
-  <si>
-    <t>LED matrix: Shielded cable</t>
-  </si>
-  <si>
-    <t>LED matrix: Panel mount</t>
-  </si>
-  <si>
     <t>LED matrix: Panel mount EMC nut</t>
   </si>
   <si>
@@ -445,9 +433,6 @@
     <t>https://nl.farnell.com/multicomp/2227mc-14-03-10-f1/socket-ic-dil-0-3-14way/dp/1103845</t>
   </si>
   <si>
-    <t>ordered 2</t>
-  </si>
-  <si>
     <t>41/56</t>
   </si>
   <si>
@@ -524,6 +509,39 @@
   </si>
   <si>
     <t>32/56</t>
+  </si>
+  <si>
+    <t>Phoenix 1440164</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/phoenix-contact/1440164/emc-nut-size-m16-m12-connector/dp/2545245</t>
+  </si>
+  <si>
+    <t>Phoenix 1404642</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/phoenix-contact/sacc-m12fss-3pecon-pg11-m/sensor-actuator-socket-m12-4pos/dp/2449313</t>
+  </si>
+  <si>
+    <t>LED matrix: Cable connector, socket</t>
+  </si>
+  <si>
+    <t>LED matrix: Panel mount, socket</t>
+  </si>
+  <si>
+    <t>LED matrix: Panel mount, plug</t>
+  </si>
+  <si>
+    <t>LED matrix: Shielded cable, plug</t>
+  </si>
+  <si>
+    <t>Phoenix 1424139</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/phoenix-contact/sacc-e-m12mss-4con-m16-0-5-pe/sensor-lead-m12-plug-4pos/dp/2449272</t>
+  </si>
+  <si>
+    <t>ordered 4</t>
   </si>
 </sst>
 </file>
@@ -978,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EABDC01-B8C9-4DFC-A32F-D1F25B52CF32}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1304,7 +1322,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>58</v>
@@ -1358,16 +1376,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E17" s="14">
         <v>25.61</v>
@@ -1380,7 +1398,7 @@
         <v>25.61</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
@@ -1388,10 +1406,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E18" s="14">
         <v>21</v>
@@ -1404,23 +1422,23 @@
         <v>42</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="7"/>
       <c r="B19" s="12"/>
       <c r="C19" s="25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
       <c r="H19" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -1428,10 +1446,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E20" s="14">
         <v>0.82</v>
@@ -1444,7 +1462,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1452,10 +1470,10 @@
         <v>40</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E21" s="14">
         <v>0.12</v>
@@ -1468,7 +1486,7 @@
         <v>3.5999999999999996</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -1477,10 +1495,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E22" s="14">
         <v>0.22</v>
@@ -1493,7 +1511,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -1523,7 +1541,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="14">
-        <f t="shared" ref="G25:G52" si="3">E25*F25</f>
+        <f t="shared" ref="G25:G54" si="3">E25*F25</f>
         <v>112</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -1556,7 +1574,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B27" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>17</v>
@@ -1580,7 +1598,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B28" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>19</v>
@@ -1657,10 +1675,10 @@
         <v>40</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E31" s="14">
         <v>2.34</v>
@@ -1673,7 +1691,7 @@
         <v>23.4</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
@@ -1701,22 +1719,22 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B33" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="B33" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="14">
         <v>82.12</v>
       </c>
-      <c r="F33" s="9">
-        <v>1</v>
-      </c>
-      <c r="G33" s="10">
+      <c r="F33" s="13">
+        <v>1</v>
+      </c>
+      <c r="G33" s="14">
         <f t="shared" si="3"/>
         <v>82.12</v>
       </c>
@@ -1725,22 +1743,22 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B34" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="B34" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="14">
         <v>16.25</v>
       </c>
-      <c r="F34" s="9">
-        <v>1</v>
-      </c>
-      <c r="G34" s="10">
+      <c r="F34" s="13">
+        <v>1</v>
+      </c>
+      <c r="G34" s="14">
         <f t="shared" si="3"/>
         <v>16.25</v>
       </c>
@@ -1749,75 +1767,75 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B35" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="18" t="s">
+      <c r="B35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="14">
+      <c r="D35" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1.27</v>
+      </c>
+      <c r="F35" s="9">
         <v>2</v>
       </c>
-      <c r="F35" s="13">
-        <v>1</v>
-      </c>
-      <c r="G35" s="14">
-        <f t="shared" si="3"/>
-        <v>2</v>
+      <c r="G35" s="10">
+        <f t="shared" si="3"/>
+        <v>2.54</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B36" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="14">
-        <v>2.59</v>
-      </c>
-      <c r="F36" s="13">
-        <v>10</v>
-      </c>
-      <c r="G36" s="14">
-        <f t="shared" si="3"/>
-        <v>25.9</v>
+      <c r="B36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="10">
+        <v>20.63</v>
+      </c>
+      <c r="F36" s="9">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10">
+        <f t="shared" si="3"/>
+        <v>20.63</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B37" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="F37" s="13">
-        <v>10</v>
-      </c>
-      <c r="G37" s="14">
-        <f t="shared" si="3"/>
-        <v>26</v>
+      <c r="B37" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="10">
+        <v>16.7</v>
+      </c>
+      <c r="F37" s="9">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10">
+        <f t="shared" si="3"/>
+        <v>16.7</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.45">
@@ -1825,23 +1843,23 @@
         <v>40</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E38" s="14">
-        <v>2.6</v>
+        <v>2.59</v>
       </c>
       <c r="F38" s="13">
         <v>10</v>
       </c>
       <c r="G38" s="14">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>25.9</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.45">
@@ -1849,23 +1867,23 @@
         <v>40</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E39" s="14">
-        <v>2.75</v>
+        <v>2.6</v>
       </c>
       <c r="F39" s="13">
         <v>10</v>
       </c>
       <c r="G39" s="14">
         <f t="shared" si="3"/>
-        <v>27.5</v>
+        <v>26</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.45">
@@ -1873,23 +1891,23 @@
         <v>40</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E40" s="14">
-        <v>0.38</v>
+        <v>2.6</v>
       </c>
       <c r="F40" s="13">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G40" s="14">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.45">
@@ -1897,23 +1915,23 @@
         <v>40</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="E41" s="14">
-        <v>7.62</v>
+        <v>2.75</v>
       </c>
       <c r="F41" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G41" s="14">
         <f t="shared" si="3"/>
-        <v>7.62</v>
+        <v>27.5</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.45">
@@ -1921,23 +1939,23 @@
         <v>40</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="E42" s="14">
-        <v>9.07</v>
+        <v>0.38</v>
       </c>
       <c r="F42" s="13">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G42" s="14">
         <f t="shared" si="3"/>
-        <v>9.07</v>
+        <v>19</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.45">
@@ -1945,23 +1963,23 @@
         <v>40</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E43" s="14">
-        <v>9.25</v>
+        <v>7.62</v>
       </c>
       <c r="F43" s="13">
         <v>1</v>
       </c>
       <c r="G43" s="14">
         <f t="shared" si="3"/>
-        <v>9.25</v>
+        <v>7.62</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.45">
@@ -1969,23 +1987,23 @@
         <v>40</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E44" s="14">
-        <v>14.17</v>
+        <v>9.07</v>
       </c>
       <c r="F44" s="13">
         <v>1</v>
       </c>
       <c r="G44" s="14">
         <f t="shared" si="3"/>
-        <v>14.17</v>
+        <v>9.07</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.45">
@@ -1993,23 +2011,23 @@
         <v>40</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E45" s="14">
-        <v>8.51</v>
+        <v>9.25</v>
       </c>
       <c r="F45" s="13">
         <v>1</v>
       </c>
       <c r="G45" s="14">
         <f t="shared" si="3"/>
-        <v>8.51</v>
+        <v>9.25</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.45">
@@ -2017,23 +2035,23 @@
         <v>40</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E46" s="14">
-        <v>6.41</v>
+        <v>14.17</v>
       </c>
       <c r="F46" s="13">
         <v>1</v>
       </c>
       <c r="G46" s="14">
         <f t="shared" si="3"/>
-        <v>6.41</v>
+        <v>14.17</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.45">
@@ -2041,23 +2059,23 @@
         <v>40</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E47" s="14">
-        <v>15.47</v>
+        <v>8.51</v>
       </c>
       <c r="F47" s="13">
         <v>1</v>
       </c>
       <c r="G47" s="14">
         <f t="shared" si="3"/>
-        <v>15.47</v>
+        <v>8.51</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.45">
@@ -2065,110 +2083,158 @@
         <v>40</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E48" s="14">
+        <v>6.41</v>
+      </c>
+      <c r="F48" s="13">
+        <v>1</v>
+      </c>
+      <c r="G48" s="14">
+        <f t="shared" si="3"/>
+        <v>6.41</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B49" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" s="14">
+        <v>15.47</v>
+      </c>
+      <c r="F49" s="13">
+        <v>1</v>
+      </c>
+      <c r="G49" s="14">
+        <f t="shared" si="3"/>
+        <v>15.47</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B50" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="14">
         <v>28.96</v>
       </c>
-      <c r="F48" s="13">
-        <v>1</v>
-      </c>
-      <c r="G48" s="14">
+      <c r="F50" s="13">
+        <v>1</v>
+      </c>
+      <c r="G50" s="14">
         <f t="shared" si="3"/>
         <v>28.96</v>
       </c>
-      <c r="H48" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B49" s="21"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H50" s="4"/>
+      <c r="H50" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A51" s="7" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="14">
+      <c r="B53" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="14">
         <v>318.16000000000003</v>
       </c>
-      <c r="F51" s="13">
-        <v>1</v>
-      </c>
-      <c r="G51" s="14">
-        <f>E51*F51</f>
-        <v>318.16000000000003</v>
-      </c>
-      <c r="H51" s="23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B52" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" s="14">
-        <v>28.5</v>
-      </c>
-      <c r="F52" s="13">
-        <v>1</v>
-      </c>
-      <c r="G52" s="14">
-        <f t="shared" si="3"/>
-        <v>28.5</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B53" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="14">
-        <v>9.83</v>
-      </c>
       <c r="F53" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G53" s="14">
         <f>E53*F53</f>
+        <v>318.16000000000003</v>
+      </c>
+      <c r="H53" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B54" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" s="14">
+        <v>28.5</v>
+      </c>
+      <c r="F54" s="13">
+        <v>1</v>
+      </c>
+      <c r="G54" s="14">
+        <f t="shared" si="3"/>
+        <v>28.5</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B55" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="14">
+        <v>9.83</v>
+      </c>
+      <c r="F55" s="13">
+        <v>3</v>
+      </c>
+      <c r="G55" s="14">
+        <f>E55*F55</f>
         <v>29.490000000000002</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>85</v>
+      <c r="H55" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2191,8 +2257,8 @@
     <hyperlink ref="H15" r:id="rId15" xr:uid="{9CE1B218-A51B-4D74-8E60-BC48A6732159}"/>
     <hyperlink ref="H29" r:id="rId16" xr:uid="{21139B33-0F0B-40A6-A529-31ED4FA41410}"/>
     <hyperlink ref="H33" r:id="rId17" xr:uid="{2FB12F3E-2615-4CE9-857F-9A7A5B1D9736}"/>
-    <hyperlink ref="H53" r:id="rId18" xr:uid="{F2F7E969-5D11-4304-BC12-98AF6A6F8DB8}"/>
-    <hyperlink ref="H52" r:id="rId19" xr:uid="{BC166A5C-E799-4B24-8CD9-D0CFD834F7A9}"/>
+    <hyperlink ref="H55" r:id="rId18" xr:uid="{F2F7E969-5D11-4304-BC12-98AF6A6F8DB8}"/>
+    <hyperlink ref="H54" r:id="rId19" xr:uid="{BC166A5C-E799-4B24-8CD9-D0CFD834F7A9}"/>
     <hyperlink ref="H31" r:id="rId20" xr:uid="{CA7C0345-0A84-4520-B968-21F94DB74B6F}"/>
     <hyperlink ref="H32" r:id="rId21" xr:uid="{98E0B643-0B27-4820-9B32-2ED486935FC0}"/>
     <hyperlink ref="H17" r:id="rId22" xr:uid="{BCE8848E-1B0B-40B8-A1F5-1B128E2593DD}"/>
@@ -2201,14 +2267,15 @@
     <hyperlink ref="H19" r:id="rId25" xr:uid="{ED7DC865-0754-4677-BBE5-BF4AF851177F}"/>
     <hyperlink ref="H22" r:id="rId26" xr:uid="{84A0CCC1-A592-4931-A941-E5326C8FC464}"/>
     <hyperlink ref="H14" r:id="rId27" xr:uid="{E15EEAD3-0BA4-4EAA-B8F8-731BE217E79B}"/>
-    <hyperlink ref="H42" r:id="rId28" xr:uid="{E27B3782-52AC-4DD1-9C40-C9CAE2CD205F}"/>
-    <hyperlink ref="H43" r:id="rId29" xr:uid="{FA68116D-962D-438B-964C-3508A341D914}"/>
-    <hyperlink ref="H44" r:id="rId30" xr:uid="{04802529-4914-4832-9CA2-2D2BD0F76FD6}"/>
-    <hyperlink ref="H45" r:id="rId31" xr:uid="{D97DA7B3-DB8B-4A29-922C-1947EA3D1DA0}"/>
+    <hyperlink ref="H44" r:id="rId28" xr:uid="{E27B3782-52AC-4DD1-9C40-C9CAE2CD205F}"/>
+    <hyperlink ref="H45" r:id="rId29" xr:uid="{FA68116D-962D-438B-964C-3508A341D914}"/>
+    <hyperlink ref="H46" r:id="rId30" xr:uid="{04802529-4914-4832-9CA2-2D2BD0F76FD6}"/>
+    <hyperlink ref="H47" r:id="rId31" xr:uid="{D97DA7B3-DB8B-4A29-922C-1947EA3D1DA0}"/>
     <hyperlink ref="H34" r:id="rId32" xr:uid="{578C99D7-4447-40EF-8C65-759B18DC19FC}"/>
-    <hyperlink ref="H46" r:id="rId33" xr:uid="{68C87FBD-315D-4D2B-BA53-B60E11432DC6}"/>
+    <hyperlink ref="H48" r:id="rId33" xr:uid="{68C87FBD-315D-4D2B-BA53-B60E11432DC6}"/>
+    <hyperlink ref="H35" r:id="rId34" xr:uid="{F2D2CBB0-73A5-4D87-8FF0-E76A17D41BDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>